<commit_message>
Edited formatting of Q1 spreadsheet
</commit_message>
<xml_diff>
--- a/Q1 Occuptional Outlook Handbook Spreadsheet.xlsx
+++ b/Q1 Occuptional Outlook Handbook Spreadsheet.xlsx
@@ -43,8 +43,7 @@
     <t>Software Developer</t>
   </si>
   <si>
-    <t>$109,020 per year
-$52.41 per hour</t>
+    <t>$109,020 per year ($52.41 per hour)</t>
   </si>
   <si>
     <t>Bachelor's degree</t>
@@ -59,8 +58,7 @@
     <t>Computer Programmer</t>
   </si>
   <si>
-    <t>$93,000 per year
-$44.71 per hour</t>
+    <t>$93,000 per year ($44.71 per hour)</t>
   </si>
   <si>
     <t>-10% (Decline)</t>
@@ -69,8 +67,7 @@
     <t>Data Scientist</t>
   </si>
   <si>
-    <t>$100,910 per year
-$48.52 per hour</t>
+    <t>$100,910 per year ($48.52 per hour)</t>
   </si>
   <si>
     <t>36% (Much faster than average)</t>
@@ -79,8 +76,7 @@
     <t>Financial Analyst</t>
   </si>
   <si>
-    <t>$95,570 per year
-$45.95 per hour</t>
+    <t>$95,570 per year ($45.95 per hour)</t>
   </si>
   <si>
     <t>9% (Faster than average)</t>
@@ -89,8 +85,7 @@
     <t>Computer Network Engineer</t>
   </si>
   <si>
-    <t>$120,520 per year
-$57.94 per hour</t>
+    <t>$120,520 per year ($57.94 per hour)</t>
   </si>
   <si>
     <t>5 years or more</t>
@@ -102,8 +97,7 @@
     <t>Computer and Information Research Scientist</t>
   </si>
   <si>
-    <t>$131,490 per year
-$63.22 per hour</t>
+    <t>$131,490 per year ($63.22 per hour)</t>
   </si>
   <si>
     <t>21% (Much faster than average)</t>
@@ -112,8 +106,7 @@
     <t>Web Developer</t>
   </si>
   <si>
-    <t>$78,300 per year
-$37.65 per hour</t>
+    <t xml:space="preserve">$78,300 per year ($37.65 per hour) </t>
   </si>
   <si>
     <t>23% (Much faster than average)</t>
@@ -122,8 +115,7 @@
     <t>Computer Hardware Engineer</t>
   </si>
   <si>
-    <t>$128,170 per year
-$61.62 per hour</t>
+    <t>$128,170 per year ($61.62 per hour)</t>
   </si>
   <si>
     <t>5% (As fast as average)</t>
@@ -132,15 +124,13 @@
     <t>Computer System Analyst</t>
   </si>
   <si>
-    <t>$99,270 per year
-$47.73 per hour</t>
+    <t>$99,270 per year ($47.73 per hour)</t>
   </si>
   <si>
     <t>Computer Support Specialist</t>
   </si>
   <si>
-    <t>$57,910 per year
-$27.84 per hour</t>
+    <t>$57,910 per year ($27.84 per hour)</t>
   </si>
   <si>
     <t>Associate's degree</t>
@@ -443,11 +433,11 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="13.5"/>
     <col customWidth="1" min="2" max="2" width="39.0"/>
-    <col customWidth="1" min="3" max="3" width="19.75"/>
+    <col customWidth="1" min="3" max="3" width="33.5"/>
     <col customWidth="1" min="4" max="4" width="26.13"/>
     <col customWidth="1" min="5" max="5" width="36.0"/>
     <col customWidth="1" min="6" max="7" width="28.5"/>
-    <col customWidth="1" min="8" max="8" width="26.75"/>
+    <col customWidth="1" min="8" max="8" width="31.63"/>
     <col customWidth="1" min="9" max="9" width="26.38"/>
   </cols>
   <sheetData>
@@ -506,7 +496,7 @@
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -698,7 +688,7 @@
       <c r="B6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -842,7 +832,7 @@
       <c r="B9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -890,7 +880,7 @@
       <c r="B10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="4" t="s">

</xml_diff>